<commit_message>
Started working on the following workflows: Main, Process, CheckOtherDeductions.
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/CountyMapping.xlsx
+++ b/STS IR Bot Performer/Data/CountyMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{7F486F02-D2CB-4EB8-A587-BE54DF2A8ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DC886D7-4686-4163-B227-6DDF9E4923E9}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{7F486F02-D2CB-4EB8-A587-BE54DF2A8ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6220341E-0EB8-413D-BB36-A82148867012}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:J178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1781,152 +1781,152 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
+        <v>224</v>
+      </c>
+      <c r="C37" t="s">
+        <v>243</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" t="s">
+        <v>224</v>
+      </c>
+      <c r="C38" t="s">
+        <v>246</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" t="s">
+        <v>224</v>
+      </c>
+      <c r="C39" t="s">
+        <v>244</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="s">
+        <v>224</v>
+      </c>
+      <c r="C40" t="s">
+        <v>243</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" t="s">
+        <v>224</v>
+      </c>
+      <c r="C41" t="s">
+        <v>194</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" t="s">
+        <v>224</v>
+      </c>
+      <c r="C42" t="s">
+        <v>243</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" t="s">
+        <v>224</v>
+      </c>
+      <c r="C43" t="s">
+        <v>243</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" t="s">
+        <v>224</v>
+      </c>
+      <c r="C44" t="s">
+        <v>244</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B45" t="s">
         <v>220</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C45" t="s">
         <v>191</v>
       </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" t="s">
-        <v>224</v>
-      </c>
-      <c r="C38" t="s">
-        <v>192</v>
-      </c>
-      <c r="D38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" t="s">
-        <v>224</v>
-      </c>
-      <c r="C39" t="s">
-        <v>193</v>
-      </c>
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" t="s">
-        <v>224</v>
-      </c>
-      <c r="C40" t="s">
-        <v>241</v>
-      </c>
-      <c r="D40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" t="s">
-        <v>224</v>
-      </c>
-      <c r="C41" t="s">
-        <v>241</v>
-      </c>
-      <c r="D41" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" t="s">
-        <v>224</v>
-      </c>
-      <c r="C42" t="s">
-        <v>242</v>
-      </c>
-      <c r="D42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" t="s">
-        <v>224</v>
-      </c>
-      <c r="C43" t="s">
-        <v>242</v>
-      </c>
-      <c r="D43" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" t="s">
-        <v>224</v>
-      </c>
-      <c r="C44" t="s">
-        <v>242</v>
-      </c>
-      <c r="D44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" t="s">
-        <v>224</v>
-      </c>
-      <c r="C45" t="s">
-        <v>243</v>
-      </c>
       <c r="D45" t="s">
         <v>6</v>
       </c>
@@ -1934,15 +1934,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
         <v>224</v>
       </c>
       <c r="C46" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
@@ -1951,15 +1951,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s">
         <v>224</v>
       </c>
       <c r="C47" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D47" t="s">
         <v>6</v>
@@ -1968,15 +1968,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s">
         <v>224</v>
       </c>
       <c r="C48" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
@@ -1985,26 +1985,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" t="s">
+        <v>224</v>
+      </c>
+      <c r="C49" t="s">
+        <v>244</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B49" t="s">
-        <v>224</v>
-      </c>
-      <c r="C49" t="s">
-        <v>243</v>
-      </c>
-      <c r="D49" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="B50" t="s">
         <v>224</v>
@@ -2019,15 +2019,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
         <v>224</v>
       </c>
       <c r="C51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D51" t="s">
         <v>6</v>
@@ -2036,15 +2036,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B52" t="s">
         <v>224</v>
       </c>
       <c r="C52" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D52" t="s">
         <v>6</v>
@@ -2053,15 +2053,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B53" t="s">
         <v>224</v>
       </c>
       <c r="C53" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D53" t="s">
         <v>6</v>
@@ -2070,15 +2070,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B54" t="s">
         <v>224</v>
       </c>
       <c r="C54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
@@ -2087,15 +2087,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B55" t="s">
         <v>224</v>
       </c>
       <c r="C55" t="s">
-        <v>243</v>
+        <v>192</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
@@ -2104,15 +2104,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="B56" t="s">
         <v>224</v>
       </c>
       <c r="C56" t="s">
-        <v>243</v>
+        <v>195</v>
       </c>
       <c r="D56" t="s">
         <v>6</v>
@@ -2121,15 +2121,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B57" t="s">
         <v>224</v>
       </c>
       <c r="C57" t="s">
-        <v>243</v>
+        <v>193</v>
       </c>
       <c r="D57" t="s">
         <v>6</v>
@@ -2138,9 +2138,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
         <v>224</v>
@@ -2155,15 +2155,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B59" t="s">
         <v>224</v>
       </c>
       <c r="C59" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D59" t="s">
         <v>6</v>
@@ -2172,15 +2172,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>65</v>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>156</v>
       </c>
       <c r="B60" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="C60" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D60" t="s">
         <v>6</v>
@@ -2189,15 +2189,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="B61" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C61" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="D61" t="s">
         <v>6</v>
@@ -2206,15 +2206,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B62" t="s">
         <v>224</v>
       </c>
       <c r="C62" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D62" t="s">
         <v>6</v>
@@ -2223,9 +2223,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B63" t="s">
         <v>224</v>
@@ -2240,15 +2240,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B64" t="s">
         <v>224</v>
       </c>
       <c r="C64" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D64" t="s">
         <v>6</v>
@@ -2257,9 +2257,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B65" t="s">
         <v>224</v>
@@ -2274,9 +2274,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B66" t="s">
         <v>224</v>
@@ -2291,15 +2291,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
         <v>224</v>
       </c>
       <c r="C67" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D67" t="s">
         <v>6</v>
@@ -2308,15 +2308,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B68" t="s">
         <v>224</v>
       </c>
       <c r="C68" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D68" t="s">
         <v>6</v>
@@ -2325,15 +2325,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="B69" t="s">
         <v>224</v>
       </c>
       <c r="C69" t="s">
-        <v>244</v>
+        <v>196</v>
       </c>
       <c r="D69" t="s">
         <v>6</v>
@@ -2342,9 +2342,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B70" t="s">
         <v>224</v>
@@ -2359,9 +2359,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
         <v>224</v>
@@ -2376,15 +2376,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B72" t="s">
         <v>224</v>
       </c>
       <c r="C72" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D72" t="s">
         <v>6</v>
@@ -2393,60 +2393,60 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B73" t="s">
+        <v>224</v>
+      </c>
+      <c r="C73" t="s">
+        <v>246</v>
+      </c>
+      <c r="D73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B74" t="s">
+        <v>224</v>
+      </c>
+      <c r="C74" t="s">
+        <v>243</v>
+      </c>
+      <c r="D74" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B75" t="s">
+        <v>224</v>
+      </c>
+      <c r="C75" t="s">
+        <v>243</v>
+      </c>
+      <c r="D75" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B73" t="s">
-        <v>224</v>
-      </c>
-      <c r="C73" t="s">
-        <v>244</v>
-      </c>
-      <c r="D73" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B74" t="s">
-        <v>224</v>
-      </c>
-      <c r="C74" t="s">
-        <v>244</v>
-      </c>
-      <c r="D74" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B75" t="s">
-        <v>224</v>
-      </c>
-      <c r="C75" t="s">
-        <v>244</v>
-      </c>
-      <c r="D75" t="s">
-        <v>6</v>
-      </c>
-      <c r="E75" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="B76" t="s">
         <v>224</v>
@@ -2461,152 +2461,152 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B77" t="s">
         <v>224</v>
       </c>
       <c r="C77" t="s">
+        <v>243</v>
+      </c>
+      <c r="D77" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B78" t="s">
+        <v>224</v>
+      </c>
+      <c r="C78" t="s">
+        <v>243</v>
+      </c>
+      <c r="D78" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>224</v>
+      </c>
+      <c r="C79" t="s">
         <v>244</v>
       </c>
-      <c r="D77" t="s">
-        <v>6</v>
-      </c>
-      <c r="E77" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B78" t="s">
-        <v>224</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="D79" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B80" t="s">
+        <v>224</v>
+      </c>
+      <c r="C80" t="s">
+        <v>243</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B81" t="s">
+        <v>224</v>
+      </c>
+      <c r="C81" t="s">
+        <v>243</v>
+      </c>
+      <c r="D81" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" t="s">
+        <v>224</v>
+      </c>
+      <c r="C82" t="s">
         <v>245</v>
       </c>
-      <c r="D78" t="s">
-        <v>6</v>
-      </c>
-      <c r="E78" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B79" t="s">
-        <v>224</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="D82" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B83" t="s">
+        <v>224</v>
+      </c>
+      <c r="C83" t="s">
+        <v>243</v>
+      </c>
+      <c r="D83" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" t="s">
+        <v>224</v>
+      </c>
+      <c r="C84" t="s">
+        <v>244</v>
+      </c>
+      <c r="D84" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>224</v>
+      </c>
+      <c r="C85" t="s">
         <v>245</v>
       </c>
-      <c r="D79" t="s">
-        <v>6</v>
-      </c>
-      <c r="E79" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B80" t="s">
-        <v>224</v>
-      </c>
-      <c r="C80" t="s">
-        <v>245</v>
-      </c>
-      <c r="D80" t="s">
-        <v>6</v>
-      </c>
-      <c r="E80" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81" t="s">
-        <v>224</v>
-      </c>
-      <c r="C81" t="s">
-        <v>246</v>
-      </c>
-      <c r="D81" t="s">
-        <v>6</v>
-      </c>
-      <c r="E81" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B82" t="s">
-        <v>224</v>
-      </c>
-      <c r="C82" t="s">
-        <v>246</v>
-      </c>
-      <c r="D82" t="s">
-        <v>6</v>
-      </c>
-      <c r="E82" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B83" t="s">
-        <v>224</v>
-      </c>
-      <c r="C83" t="s">
-        <v>246</v>
-      </c>
-      <c r="D83" t="s">
-        <v>6</v>
-      </c>
-      <c r="E83" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84" t="s">
-        <v>224</v>
-      </c>
-      <c r="C84" t="s">
-        <v>246</v>
-      </c>
-      <c r="D84" t="s">
-        <v>6</v>
-      </c>
-      <c r="E84" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B85" t="s">
-        <v>224</v>
-      </c>
-      <c r="C85" t="s">
-        <v>194</v>
-      </c>
       <c r="D85" t="s">
         <v>6</v>
       </c>
@@ -2614,15 +2614,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B86" t="s">
         <v>224</v>
       </c>
       <c r="C86" t="s">
-        <v>195</v>
+        <v>244</v>
       </c>
       <c r="D86" t="s">
         <v>6</v>
@@ -2631,15 +2631,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B87" t="s">
         <v>224</v>
       </c>
       <c r="C87" t="s">
-        <v>196</v>
+        <v>243</v>
       </c>
       <c r="D87" t="s">
         <v>6</v>
@@ -3719,7 +3719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>154</v>
       </c>
@@ -3753,15 +3753,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>156</v>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B153" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C153" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="D153" t="s">
         <v>6</v>
@@ -3770,15 +3770,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>157</v>
+        <v>68</v>
       </c>
       <c r="B154" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C154" t="s">
-        <v>202</v>
+        <v>243</v>
       </c>
       <c r="D154" t="s">
         <v>6</v>
@@ -4199,9 +4199,63 @@
   <autoFilter ref="A1:E178" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="AR ET-1"/>
+        <filter val="CO Arvada ST"/>
+        <filter val="CO Aspen"/>
+        <filter val="CO Aurora"/>
+        <filter val="CO Avon"/>
+        <filter val="CO Black Hawk"/>
+        <filter val="CO Boulder"/>
+        <filter val="CO Breckenridge"/>
+        <filter val="CO Brighton ST"/>
+        <filter val="CO Broomfield"/>
+        <filter val="CO Carbondale"/>
+        <filter val="CO Castle Pines"/>
+        <filter val="CO Castle Rock ST"/>
+        <filter val="CO Centennial"/>
+        <filter val="CO Central ST"/>
+        <filter val="CO Cherry Hills"/>
+        <filter val="CO Colorado Springs"/>
+        <filter val="CO Commerce"/>
+        <filter val="CO Cortez"/>
+        <filter val="CO Craig"/>
+        <filter val="CO Crested Butte"/>
+        <filter val="CO Dacono"/>
+        <filter val="CO Delta ST"/>
+        <filter val="CO Denver 100"/>
+        <filter val="CO DR-0100 XML"/>
+        <filter val="CO DR-0173"/>
+        <filter val="CO Durango"/>
+        <filter val="CO Edgewater"/>
+        <filter val="CO Englewood"/>
+        <filter val="CO Evans"/>
+        <filter val="CO Federal HGTS ST"/>
+        <filter val="CO Fort Collins"/>
+        <filter val="CO Frisco"/>
+        <filter val="CO Glendale"/>
+        <filter val="CO Glenwood Spr ST"/>
+        <filter val="CO Golden"/>
+        <filter val="CO Grand Junction"/>
+        <filter val="CO Greeley"/>
+        <filter val="CO Greenwood Village"/>
+        <filter val="CO La Junta"/>
+        <filter val="CO Lafayette"/>
+        <filter val="CO Lakewood"/>
+        <filter val="CO Littleton"/>
+        <filter val="CO Longmont ST"/>
+        <filter val="CO Louisville ST"/>
+        <filter val="CO Loveland"/>
+        <filter val="CO Montrose"/>
+        <filter val="CO Parket ST"/>
+        <filter val="CO Pueblo"/>
+        <filter val="CO Thornton ST"/>
+        <filter val="CO Westminster ST"/>
+        <filter val="CO Wheat Ridge"/>
+        <filter val="CO Woodland"/>
       </filters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A37:E154">
+      <sortCondition ref="A1:A178"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>